<commit_message>
Correção ao use case Configuração Inicial
</commit_message>
<xml_diff>
--- a/Parte2/use_cases/Configuração Inicial.xlsx
+++ b/Parte2/use_cases/Configuração Inicial.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6C1F9C-C278-4F68-A574-5347274FA9A8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633F7C68-8E41-45F7-B160-C7E43C69356B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2895" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,15 +57,6 @@
 do utilizador.</t>
   </si>
   <si>
-    <t>Alternativa 1 [Não existem receitas para a combinação definida] (Passo 3)</t>
-  </si>
-  <si>
-    <t>3.1 Informa que não existem receitas para a configuração</t>
-  </si>
-  <si>
-    <t>3.2 Regressa ao Passo 1</t>
-  </si>
-  <si>
     <t>5. Regista a configuração</t>
   </si>
   <si>
@@ -73,21 +64,28 @@
 utilizador quer alterar a configuração] (Passo 4)</t>
   </si>
   <si>
-    <t>4.2 Regressa ao passo 3</t>
-  </si>
-  <si>
-    <t>1. Apresenta as opções para selecionar com os 
-ingredientes/temperatura preferida 
-(3 ingredientes, 1 temperatura)</t>
-  </si>
-  <si>
-    <t>2. Indica as opções escolhidas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. Indica que quer terminar a Configuração Inicial  </t>
-  </si>
-  <si>
     <t>4.1 Indica as alterações a efetuar</t>
+  </si>
+  <si>
+    <t>1. Apresenta as opções de seleção dos ingredientes e temperatura preferidos</t>
+  </si>
+  <si>
+    <t>2. Seleciona ingredientes/temperatura</t>
+  </si>
+  <si>
+    <t>Alternativa 1 [Não existem receitas para a combinação definida] (Passo 2)</t>
+  </si>
+  <si>
+    <t>2.1 Informa que não existem receitas para a configuração</t>
+  </si>
+  <si>
+    <t>2.2 Regressa ao Passo 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Termina a Configuração Inicial  </t>
+  </si>
+  <si>
+    <t>4.2 Regressa ao passo 1</t>
   </si>
 </sst>
 </file>
@@ -711,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,17 +765,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="25"/>
       <c r="B6" s="4"/>
       <c r="C6" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25"/>
       <c r="B7" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" s="5"/>
     </row>
@@ -799,7 +797,7 @@
       <c r="A10" s="25"/>
       <c r="B10" s="4"/>
       <c r="C10" s="12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -809,18 +807,18 @@
     </row>
     <row r="12" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="25"/>
       <c r="B13" s="4"/>
       <c r="C13" s="11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -830,10 +828,10 @@
     </row>
     <row r="15" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C15" s="15"/>
     </row>
@@ -841,7 +839,7 @@
       <c r="A16" s="21"/>
       <c r="B16" s="13"/>
       <c r="C16" s="19" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adicionada uma porrada de modelos, bem como prints de alguns use_cases que já estão no relatório
</commit_message>
<xml_diff>
--- a/Parte2/use_cases/Configuração Inicial.xlsx
+++ b/Parte2/use_cases/Configuração Inicial.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633F7C68-8E41-45F7-B160-C7E43C69356B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96876C9-1878-4892-A48D-4152B9A14D54}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,6 @@
     <t>Actor:</t>
   </si>
   <si>
-    <t>Utilizador</t>
-  </si>
-  <si>
     <t>Pré condição:</t>
   </si>
   <si>
@@ -60,32 +57,35 @@
     <t>5. Regista a configuração</t>
   </si>
   <si>
+    <t>1. Apresenta as opções de seleção dos ingredientes e temperatura preferidos</t>
+  </si>
+  <si>
+    <t>2. Seleciona ingredientes/temperatura</t>
+  </si>
+  <si>
+    <t>Alternativa 1 [Não existem receitas para a combinação definida] (Passo 2)</t>
+  </si>
+  <si>
+    <t>2.1 Informa que não existem receitas para a configuração</t>
+  </si>
+  <si>
+    <t>2.2 Regressa ao Passo 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Termina a Configuração Inicial  </t>
+  </si>
+  <si>
+    <t>Utilizador autenticado</t>
+  </si>
+  <si>
     <t>Alternativa 2 [O
-utilizador quer alterar a configuração] (Passo 4)</t>
-  </si>
-  <si>
-    <t>4.1 Indica as alterações a efetuar</t>
-  </si>
-  <si>
-    <t>1. Apresenta as opções de seleção dos ingredientes e temperatura preferidos</t>
-  </si>
-  <si>
-    <t>2. Seleciona ingredientes/temperatura</t>
-  </si>
-  <si>
-    <t>Alternativa 1 [Não existem receitas para a combinação definida] (Passo 2)</t>
-  </si>
-  <si>
-    <t>2.1 Informa que não existem receitas para a configuração</t>
-  </si>
-  <si>
-    <t>2.2 Regressa ao Passo 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. Termina a Configuração Inicial  </t>
-  </si>
-  <si>
-    <t>4.2 Regressa ao passo 1</t>
+utilizador quer alterar a configuração] (Passo 3)</t>
+  </si>
+  <si>
+    <t>3.1 Indica as alterações a efetuar</t>
+  </si>
+  <si>
+    <t>3.2 Regressa ao passo 1</t>
   </si>
 </sst>
 </file>
@@ -101,18 +101,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -135,25 +133,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -380,51 +365,53 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -707,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C17" sqref="A1:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,146 +707,136 @@
     <col min="3" max="3" width="64.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="23"/>
-    </row>
-    <row r="2" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="23"/>
-    </row>
-    <row r="3" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-    </row>
-    <row r="4" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="14"/>
+    </row>
+    <row r="8" spans="1:3" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="24"/>
-    </row>
-    <row r="5" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="25"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="12" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="16"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+    </row>
+    <row r="12" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="25"/>
-      <c r="B7" s="4" t="s">
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="25"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="25"/>
-      <c r="B9" s="6" t="s">
+    </row>
+    <row r="14" spans="1:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
+    </row>
+    <row r="15" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="11"/>
-    </row>
-    <row r="10" spans="1:3" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="25"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="25"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="25"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="25"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="15"/>
-    </row>
-    <row r="16" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="19" t="s">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="16"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="16"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="17"/>
+    <row r="17" spans="1:3" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="25"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A15:A17"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>

</xml_diff>

<commit_message>
Started part 3, and added mockups from part 2
</commit_message>
<xml_diff>
--- a/Parte2/use_cases/Configuração Inicial.xlsx
+++ b/Parte2/use_cases/Configuração Inicial.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96876C9-1878-4892-A48D-4152B9A14D54}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A34D6CC-3023-4AB9-98FD-71915DE14FA9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Use Case:</t>
   </si>
@@ -82,10 +82,7 @@
 utilizador quer alterar a configuração] (Passo 3)</t>
   </si>
   <si>
-    <t>3.1 Indica as alterações a efetuar</t>
-  </si>
-  <si>
-    <t>3.2 Regressa ao passo 1</t>
+    <t>3.1 Regressa a 2</t>
   </si>
 </sst>
 </file>
@@ -365,21 +362,12 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -397,22 +385,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,7 +694,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C17" sqref="A1:C17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,131 +705,129 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="22"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="23"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="24"/>
+      <c r="B7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="11"/>
     </row>
     <row r="8" spans="1:3" ht="30" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="24"/>
+      <c r="B9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="13"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
     </row>
     <row r="12" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="21" t="s">
+      <c r="B12" s="16"/>
+      <c r="C12" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="16" t="s">
+      <c r="A13" s="25"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
     </row>
     <row r="15" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="18"/>
+      <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="A16" s="20"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="25"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>